<commit_message>
Fixed pandas import error with time series data. Added spreadsheet protection to sample grid.
</commit_message>
<xml_diff>
--- a/sample grid.xlsx
+++ b/sample grid.xlsx
@@ -2,22 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miko\Desktop\PROGRAMMING\excel grid to xml.tv\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miko\Desktop\PROGRAMMING\excel grid to xml.tv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918A1BE1-6E07-4031-BDA5-8C9FB4FB42DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6134924D-F559-4C3C-97E1-6DA7872A6F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="38520" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="38520" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Channel 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$1:$L$58</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="89">
   <si>
     <t>Channel Name</t>
   </si>
@@ -301,6 +299,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,8 +339,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -691,13 +692,13 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -752,16 +753,16 @@
       <c r="A2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>45109</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F2" t="s">
@@ -784,16 +785,16 @@
       <c r="A3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>45109</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.41666666666666669</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F3" t="s">
@@ -811,24 +812,21 @@
       <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>45109</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F4" t="s">
@@ -851,16 +849,16 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>45109</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.625</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F5" t="s">
@@ -878,27 +876,21 @@
       <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>45109</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.70833333333333337</v>
       </c>
       <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F6" t="s">
@@ -921,16 +913,16 @@
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>45109</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.79166666666666663</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F7" t="s">
@@ -953,16 +945,16 @@
       <c r="A8" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>45109</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.91666666666666663</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F8" t="s">
@@ -985,16 +977,16 @@
       <c r="A9" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>45110</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F9" t="s">
@@ -1017,16 +1009,16 @@
       <c r="A10" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>45110</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.64583333333333337</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F10" t="s">
@@ -1044,21 +1036,27 @@
       <c r="J10" t="s">
         <v>21</v>
       </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>45110</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.72916666666666663</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F11" t="s">
@@ -1076,21 +1074,27 @@
       <c r="J11" t="s">
         <v>16</v>
       </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>45110</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.83333333333333337</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F12" t="s">
@@ -1119,16 +1123,16 @@
       <c r="A13" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>45110</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.9375</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F13" t="s">
@@ -1146,21 +1150,27 @@
       <c r="J13" t="s">
         <v>25</v>
       </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>45111</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.375</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F14" t="s">
@@ -1178,21 +1188,27 @@
       <c r="J14" t="s">
         <v>16</v>
       </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>45111</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.47916666666666669</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F15" t="s">
@@ -1210,21 +1226,24 @@
       <c r="J15" t="s">
         <v>19</v>
       </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>45111</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F16" t="s">
@@ -1243,20 +1262,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>45111</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F17" t="s">
@@ -1274,24 +1293,21 @@
       <c r="J17" t="s">
         <v>16</v>
       </c>
-      <c r="K17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>45111</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.79166666666666663</v>
       </c>
       <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F18" t="s">
@@ -1310,20 +1326,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>45111</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>0.89583333333333337</v>
       </c>
       <c r="D19" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F19" t="s">
@@ -1342,20 +1358,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>45112</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0.35416666666666669</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F20" t="s">
@@ -1374,20 +1390,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>45112</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>0.45833333333333331</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F21" t="s">
@@ -1405,24 +1421,21 @@
       <c r="J21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>45112</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="D22" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F22" t="s">
@@ -1440,21 +1453,24 @@
       <c r="J22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>45112</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F23" t="s">
@@ -1472,21 +1488,24 @@
       <c r="J23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>45112</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>0.75</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F24" t="s">
@@ -1504,21 +1523,24 @@
       <c r="J24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>45112</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>0.85416666666666663</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F25" t="s">
@@ -1536,21 +1558,24 @@
       <c r="J25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>45112</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>0.95833333333333337</v>
       </c>
       <c r="D26" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F26" t="s">
@@ -1568,21 +1593,24 @@
       <c r="J26" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>45113</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>0.41666666666666669</v>
       </c>
       <c r="D27" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F27" t="s">
@@ -1600,21 +1628,24 @@
       <c r="J27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>45113</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>0.5</v>
       </c>
       <c r="D28" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F28" t="s">
@@ -1632,21 +1663,24 @@
       <c r="J28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>45113</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F29" t="s">
@@ -1664,21 +1698,24 @@
       <c r="J29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>45113</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>0.70833333333333337</v>
       </c>
       <c r="D30" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F30" t="s">
@@ -1696,21 +1733,24 @@
       <c r="J30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>45113</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>0.8125</v>
       </c>
       <c r="D31" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>0.10416666666666667</v>
       </c>
       <c r="F31" t="s">
@@ -1728,21 +1768,24 @@
       <c r="J31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>45113</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>0.9375</v>
       </c>
       <c r="D32" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F32" t="s">
@@ -1760,21 +1803,24 @@
       <c r="J32" t="s">
         <v>25</v>
       </c>
+      <c r="K32" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>45114</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="D33" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>0.10416666666666667</v>
       </c>
       <c r="F33" t="s">
@@ -1792,21 +1838,24 @@
       <c r="J33" t="s">
         <v>16</v>
       </c>
+      <c r="K33" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>45114</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>0.4375</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F34" t="s">
@@ -1824,21 +1873,24 @@
       <c r="J34" t="s">
         <v>19</v>
       </c>
+      <c r="K34" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>45114</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="D35" t="s">
         <v>62</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F35" t="s">
@@ -1856,6 +1908,9 @@
       <c r="J35" t="s">
         <v>25</v>
       </c>
+      <c r="K35" t="s">
+        <v>17</v>
+      </c>
       <c r="L35" t="s">
         <v>17</v>
       </c>
@@ -1864,16 +1919,16 @@
       <c r="A36" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>45114</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F36" t="s">
@@ -1891,21 +1946,27 @@
       <c r="J36" t="s">
         <v>25</v>
       </c>
+      <c r="K36" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>45114</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>0.75</v>
       </c>
       <c r="D37" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F37" t="s">
@@ -1923,21 +1984,27 @@
       <c r="J37" t="s">
         <v>16</v>
       </c>
+      <c r="K37" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>45114</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>0.85416666666666663</v>
       </c>
       <c r="D38" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>0.10416666666666667</v>
       </c>
       <c r="F38" t="s">
@@ -1958,21 +2025,24 @@
       <c r="K38" t="s">
         <v>17</v>
       </c>
+      <c r="L38" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>45114</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>0.95833333333333337</v>
       </c>
       <c r="D39" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F39" t="s">
@@ -1998,16 +2068,16 @@
       <c r="A40" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>45115</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>0.375</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F40" t="s">
@@ -2030,16 +2100,16 @@
       <c r="A41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>45115</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>0.45833333333333331</v>
       </c>
       <c r="D41" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F41" t="s">
@@ -2062,16 +2132,16 @@
       <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>45115</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="D42" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F42" t="s">
@@ -2094,16 +2164,16 @@
       <c r="A43" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>45115</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F43" t="s">
@@ -2126,16 +2196,16 @@
       <c r="A44" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>45115</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>0.75</v>
       </c>
       <c r="D44" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F44" t="s">
@@ -2158,16 +2228,16 @@
       <c r="A45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>45115</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>0.85416666666666663</v>
       </c>
       <c r="D45" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F45" t="s">
@@ -2190,16 +2260,16 @@
       <c r="A46" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>45115</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>0.95833333333333337</v>
       </c>
       <c r="D46" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="F46" t="s">
@@ -2217,21 +2287,24 @@
       <c r="J46" t="s">
         <v>19</v>
       </c>
+      <c r="K46" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>45116</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>0.35416666666666669</v>
       </c>
       <c r="D47" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F47" t="s">
@@ -2257,16 +2330,16 @@
       <c r="A48" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>45116</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>0.4375</v>
       </c>
       <c r="D48" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F48" t="s">
@@ -2284,21 +2357,24 @@
       <c r="J48" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>45116</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="D49" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F49" t="s">
@@ -2316,21 +2392,24 @@
       <c r="J49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>45116</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>0.625</v>
       </c>
       <c r="D50" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F50" t="s">
@@ -2348,21 +2427,24 @@
       <c r="J50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>45116</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>0.72916666666666663</v>
       </c>
       <c r="D51" t="s">
         <v>79</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F51" t="s">
@@ -2380,21 +2462,24 @@
       <c r="J51" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>45116</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>0.83333333333333337</v>
       </c>
       <c r="D52" t="s">
         <v>80</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="F52" t="s">
@@ -2415,24 +2500,21 @@
       <c r="K52" t="s">
         <v>17</v>
       </c>
-      <c r="L52" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>45116</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>0.91666666666666663</v>
       </c>
       <c r="D53" t="s">
         <v>81</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F53" t="s">
@@ -2450,21 +2532,24 @@
       <c r="J53" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>45117</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="D54" t="s">
         <v>82</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F54" t="s">
@@ -2482,21 +2567,24 @@
       <c r="J54" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>45117</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>0.64583333333333337</v>
       </c>
       <c r="D55" t="s">
         <v>83</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="1">
         <v>6.25E-2</v>
       </c>
       <c r="F55" t="s">
@@ -2514,21 +2602,24 @@
       <c r="J55" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>45117</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>0.72916666666666663</v>
       </c>
       <c r="D56" t="s">
         <v>84</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F56" t="s">
@@ -2546,21 +2637,24 @@
       <c r="J56" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>45117</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>0.83333333333333337</v>
       </c>
       <c r="D57" t="s">
         <v>85</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F57" t="s">
@@ -2581,24 +2675,21 @@
       <c r="K57" t="s">
         <v>17</v>
       </c>
-      <c r="L57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>45117</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>0.91666666666666663</v>
       </c>
       <c r="D58" t="s">
         <v>86</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F58" t="s">
@@ -2616,9 +2707,11 @@
       <c r="J58" t="s">
         <v>87</v>
       </c>
+      <c r="K58" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L58" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>